<commit_message>
Mettre à  jour la correction pour Eslint
</commit_message>
<xml_diff>
--- a/Equipe304.xlsx
+++ b/Equipe304.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26405"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikolay\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1287" documentId="13_ncr:1_{89A5CB98-93EB-451E-A012-FBFD01AD492F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{456F4389-7E3D-473F-B192-50FA9B74CE90}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DB4D43E5-522B-4F4C-9D56-ACDCF19F0778}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" firstSheet="2" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sommaire" sheetId="9" r:id="rId1"/>
@@ -374,8 +374,7 @@
 </t>
   </si>
   <si>
-    <t>src\app\pages\creation-page\creation-page.component.ts: /* eslint-disable max-lines */
-src\app\services\pop-up\pop-up.service.ts:     // eslint-disable-next-line @typescript-eslint/no-explicit-any</t>
+    <t>src\app\services\pop-up\pop-up.service.ts:     // eslint-disable-next-line @typescript-eslint/no-explicit-any</t>
   </si>
   <si>
     <t>7.7 Complexité</t>
@@ -2454,6 +2453,30 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="56" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2466,6 +2489,84 @@
     <xf numFmtId="49" fontId="13" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="8" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="8" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="8" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="9" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="9" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="9" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="10" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="10" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="10" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="17" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2475,108 +2576,6 @@
     <xf numFmtId="0" fontId="12" fillId="17" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="13" fillId="8" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="13" fillId="8" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="13" fillId="8" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="13" fillId="9" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="13" fillId="9" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="13" fillId="9" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="13" fillId="10" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="13" fillId="10" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="13" fillId="10" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2615,13 +2614,13 @@
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="40% - Accent1" xfId="4" builtinId="31"/>
-    <cellStyle name="40% - Accent2" xfId="5" builtinId="35"/>
-    <cellStyle name="40% - Accent3" xfId="6" builtinId="39"/>
-    <cellStyle name="Explanatory Text" xfId="2" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent1" xfId="4" builtinId="31"/>
+    <cellStyle name="40 % - Accent2" xfId="5" builtinId="35"/>
+    <cellStyle name="40 % - Accent3" xfId="6" builtinId="39"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Output" xfId="3" builtinId="21"/>
-    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
+    <cellStyle name="Pourcentage" xfId="1" builtinId="5"/>
+    <cellStyle name="Sortie" xfId="3" builtinId="21"/>
+    <cellStyle name="Texte explicatif" xfId="2" builtinId="53" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3078,11 +3077,11 @@
       </c>
       <c r="C5" s="113">
         <f>'Assurance Qualité'!F59</f>
-        <v>0.72750000000000004</v>
+        <v>0.74750000000000005</v>
       </c>
       <c r="D5" s="113">
         <f t="shared" ref="D5:D6" si="0">B5*0.6+C5*0.4 - 0.1*E5</f>
-        <v>0.88140000000000007</v>
+        <v>0.88940000000000008</v>
       </c>
       <c r="E5" s="114"/>
       <c r="F5" s="115">
@@ -3090,7 +3089,7 @@
       </c>
       <c r="G5" s="116">
         <f t="shared" ref="G5:G7" si="1">D5*F5</f>
-        <v>17.628</v>
+        <v>17.788</v>
       </c>
       <c r="H5" s="116">
         <f>AVERAGE(Documents!B18,Documents!F18)*5</f>
@@ -3155,8 +3154,8 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A2:Q59"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+    <sheetView tabSelected="1" topLeftCell="B44" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -3175,36 +3174,36 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:17" ht="18.399999999999999" customHeight="1">
-      <c r="A2" s="274" t="s">
+      <c r="A2" s="242" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="274"/>
-      <c r="C2" s="274"/>
-      <c r="D2" s="274"/>
-      <c r="E2" s="274"/>
-      <c r="F2" s="274"/>
-      <c r="G2" s="274"/>
-      <c r="H2" s="274"/>
-      <c r="I2" s="274"/>
-      <c r="J2" s="274"/>
-      <c r="K2" s="274"/>
+      <c r="B2" s="242"/>
+      <c r="C2" s="242"/>
+      <c r="D2" s="242"/>
+      <c r="E2" s="242"/>
+      <c r="F2" s="242"/>
+      <c r="G2" s="242"/>
+      <c r="H2" s="242"/>
+      <c r="I2" s="242"/>
+      <c r="J2" s="242"/>
+      <c r="K2" s="242"/>
       <c r="L2" s="7"/>
       <c r="M2" s="7"/>
     </row>
     <row r="4" spans="1:17" ht="18.399999999999999" customHeight="1">
-      <c r="A4" s="275" t="s">
+      <c r="A4" s="243" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="275"/>
-      <c r="C4" s="275"/>
-      <c r="D4" s="275"/>
-      <c r="E4" s="275"/>
-      <c r="F4" s="275"/>
-      <c r="G4" s="275"/>
-      <c r="H4" s="275"/>
-      <c r="I4" s="275"/>
-      <c r="J4" s="275"/>
-      <c r="K4" s="275"/>
+      <c r="B4" s="243"/>
+      <c r="C4" s="243"/>
+      <c r="D4" s="243"/>
+      <c r="E4" s="243"/>
+      <c r="F4" s="243"/>
+      <c r="G4" s="243"/>
+      <c r="H4" s="243"/>
+      <c r="I4" s="243"/>
+      <c r="J4" s="243"/>
+      <c r="K4" s="243"/>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
     </row>
@@ -3224,36 +3223,36 @@
       <c r="M5" s="2"/>
     </row>
     <row r="6" spans="1:17" ht="18.399999999999999" customHeight="1">
-      <c r="A6" s="267" t="s">
+      <c r="A6" s="260" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="279" t="s">
+      <c r="B6" s="247" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="269" t="s">
+      <c r="C6" s="262" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="270"/>
-      <c r="E6" s="270"/>
-      <c r="F6" s="271" t="s">
+      <c r="D6" s="263"/>
+      <c r="E6" s="263"/>
+      <c r="F6" s="264" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="272"/>
-      <c r="H6" s="273"/>
-      <c r="I6" s="276" t="s">
+      <c r="G6" s="265"/>
+      <c r="H6" s="266"/>
+      <c r="I6" s="244" t="s">
         <v>9</v>
       </c>
-      <c r="J6" s="277"/>
-      <c r="K6" s="278"/>
+      <c r="J6" s="245"/>
+      <c r="K6" s="246"/>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
-      <c r="N6" s="265"/>
-      <c r="O6" s="266"/>
-      <c r="P6" s="266"/>
+      <c r="N6" s="258"/>
+      <c r="O6" s="259"/>
+      <c r="P6" s="259"/>
     </row>
     <row r="7" spans="1:17" ht="18.75">
-      <c r="A7" s="268"/>
-      <c r="B7" s="280"/>
+      <c r="A7" s="261"/>
+      <c r="B7" s="248"/>
       <c r="C7" s="14" t="s">
         <v>15</v>
       </c>
@@ -3289,28 +3288,28 @@
       <c r="Q7" s="40"/>
     </row>
     <row r="8" spans="1:17" ht="18.75">
-      <c r="A8" s="249" t="s">
+      <c r="A8" s="257" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="249"/>
-      <c r="C8" s="242" t="s">
+      <c r="B8" s="257"/>
+      <c r="C8" s="250" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="243"/>
+      <c r="D8" s="251"/>
       <c r="E8" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="242" t="s">
+      <c r="F8" s="250" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="243"/>
+      <c r="G8" s="251"/>
       <c r="H8" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="I8" s="242" t="s">
+      <c r="I8" s="250" t="s">
         <v>18</v>
       </c>
-      <c r="J8" s="243"/>
+      <c r="J8" s="251"/>
       <c r="K8" s="46"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
@@ -3390,10 +3389,10 @@
       <c r="Q10" s="40"/>
     </row>
     <row r="11" spans="1:17" s="30" customFormat="1" ht="15.75">
-      <c r="A11" s="244" t="s">
+      <c r="A11" s="252" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="245"/>
+      <c r="B11" s="253"/>
       <c r="C11" s="47">
         <f>SUMPRODUCT(C6:C10,D6:D10)</f>
         <v>7.4</v>
@@ -3429,28 +3428,28 @@
       <c r="Q11" s="44"/>
     </row>
     <row r="12" spans="1:17" s="12" customFormat="1" ht="18.399999999999999" customHeight="1">
-      <c r="A12" s="249" t="s">
+      <c r="A12" s="257" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="249"/>
-      <c r="C12" s="242" t="s">
+      <c r="B12" s="257"/>
+      <c r="C12" s="250" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="243"/>
+      <c r="D12" s="251"/>
       <c r="E12" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="242" t="s">
+      <c r="F12" s="250" t="s">
         <v>18</v>
       </c>
-      <c r="G12" s="243"/>
+      <c r="G12" s="251"/>
       <c r="H12" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="I12" s="242" t="s">
+      <c r="I12" s="250" t="s">
         <v>18</v>
       </c>
-      <c r="J12" s="243"/>
+      <c r="J12" s="251"/>
       <c r="K12" s="46"/>
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
@@ -3629,10 +3628,10 @@
       <c r="M17" s="5"/>
     </row>
     <row r="18" spans="1:17" s="30" customFormat="1" ht="15.75">
-      <c r="A18" s="244" t="s">
+      <c r="A18" s="252" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="245"/>
+      <c r="B18" s="253"/>
       <c r="C18" s="47">
         <f>SUMPRODUCT(C13:C17,D13:D17)</f>
         <v>11.25</v>
@@ -3668,28 +3667,28 @@
       <c r="Q18" s="44"/>
     </row>
     <row r="19" spans="1:17" s="43" customFormat="1" ht="18.399999999999999" customHeight="1">
-      <c r="A19" s="281" t="s">
+      <c r="A19" s="249" t="s">
         <v>45</v>
       </c>
-      <c r="B19" s="281"/>
-      <c r="C19" s="242" t="s">
+      <c r="B19" s="249"/>
+      <c r="C19" s="250" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="243"/>
+      <c r="D19" s="251"/>
       <c r="E19" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="F19" s="242" t="s">
+      <c r="F19" s="250" t="s">
         <v>18</v>
       </c>
-      <c r="G19" s="243"/>
+      <c r="G19" s="251"/>
       <c r="H19" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="I19" s="242" t="s">
+      <c r="I19" s="250" t="s">
         <v>18</v>
       </c>
-      <c r="J19" s="243"/>
+      <c r="J19" s="251"/>
       <c r="K19" s="46"/>
       <c r="L19" s="4"/>
       <c r="M19" s="4"/>
@@ -3757,10 +3756,10 @@
       <c r="M21" s="5"/>
     </row>
     <row r="22" spans="1:17" s="44" customFormat="1" ht="15.75">
-      <c r="A22" s="282" t="s">
+      <c r="A22" s="254" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="264"/>
+      <c r="B22" s="255"/>
       <c r="C22" s="57">
         <f>SUMPRODUCT(C20:C21,D20:D21)</f>
         <v>5.25</v>
@@ -3796,24 +3795,24 @@
         <v>51</v>
       </c>
       <c r="B23" s="214"/>
-      <c r="C23" s="242" t="s">
+      <c r="C23" s="250" t="s">
         <v>18</v>
       </c>
-      <c r="D23" s="243"/>
+      <c r="D23" s="251"/>
       <c r="E23" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="F23" s="242" t="s">
+      <c r="F23" s="250" t="s">
         <v>18</v>
       </c>
-      <c r="G23" s="243"/>
+      <c r="G23" s="251"/>
       <c r="H23" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="I23" s="242" t="s">
+      <c r="I23" s="250" t="s">
         <v>18</v>
       </c>
-      <c r="J23" s="243"/>
+      <c r="J23" s="251"/>
       <c r="K23" s="46"/>
       <c r="L23" s="4"/>
       <c r="M23" s="4"/>
@@ -3910,10 +3909,10 @@
       <c r="M26" s="5"/>
     </row>
     <row r="27" spans="1:17" s="44" customFormat="1" ht="15.75">
-      <c r="A27" s="263" t="s">
+      <c r="A27" s="256" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="264"/>
+      <c r="B27" s="255"/>
       <c r="C27" s="47">
         <f>SUMPRODUCT(C24:C26,D24:D26)</f>
         <v>2</v>
@@ -3945,28 +3944,28 @@
       <c r="M27" s="56"/>
     </row>
     <row r="28" spans="1:17" ht="21" customHeight="1">
-      <c r="A28" s="281" t="s">
+      <c r="A28" s="249" t="s">
         <v>59</v>
       </c>
-      <c r="B28" s="281"/>
-      <c r="C28" s="242" t="s">
+      <c r="B28" s="249"/>
+      <c r="C28" s="250" t="s">
         <v>18</v>
       </c>
-      <c r="D28" s="243"/>
+      <c r="D28" s="251"/>
       <c r="E28" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="F28" s="242" t="s">
+      <c r="F28" s="250" t="s">
         <v>18</v>
       </c>
-      <c r="G28" s="243"/>
+      <c r="G28" s="251"/>
       <c r="H28" s="66" t="s">
         <v>60</v>
       </c>
-      <c r="I28" s="242" t="s">
+      <c r="I28" s="250" t="s">
         <v>18</v>
       </c>
-      <c r="J28" s="243"/>
+      <c r="J28" s="251"/>
       <c r="K28" s="46"/>
       <c r="L28" s="9"/>
       <c r="M28" s="4"/>
@@ -4073,10 +4072,10 @@
       <c r="M31" s="5"/>
     </row>
     <row r="32" spans="1:17" s="44" customFormat="1" ht="15.75">
-      <c r="A32" s="244" t="s">
+      <c r="A32" s="252" t="s">
         <v>26</v>
       </c>
-      <c r="B32" s="245"/>
+      <c r="B32" s="253"/>
       <c r="C32" s="47">
         <f>SUMPRODUCT(C29:C31,D29:D31)</f>
         <v>4</v>
@@ -4108,21 +4107,21 @@
       <c r="M32" s="56"/>
     </row>
     <row r="33" spans="1:13" ht="18.75" customHeight="1">
-      <c r="A33" s="249" t="s">
+      <c r="A33" s="257" t="s">
         <v>71</v>
       </c>
-      <c r="B33" s="249"/>
-      <c r="C33" s="242" t="s">
+      <c r="B33" s="257"/>
+      <c r="C33" s="250" t="s">
         <v>18</v>
       </c>
-      <c r="D33" s="243"/>
+      <c r="D33" s="251"/>
       <c r="E33" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="F33" s="242" t="s">
+      <c r="F33" s="250" t="s">
         <v>18</v>
       </c>
-      <c r="G33" s="243"/>
+      <c r="G33" s="251"/>
       <c r="H33" s="46" t="s">
         <v>60</v>
       </c>
@@ -4261,10 +4260,10 @@
       <c r="M37" s="5"/>
     </row>
     <row r="38" spans="1:13" s="44" customFormat="1" ht="15.75">
-      <c r="A38" s="244" t="s">
+      <c r="A38" s="252" t="s">
         <v>26</v>
       </c>
-      <c r="B38" s="245"/>
+      <c r="B38" s="253"/>
       <c r="C38" s="69">
         <f>SUMPRODUCT(C34:C37,D34:D37)</f>
         <v>5</v>
@@ -4300,24 +4299,24 @@
         <v>85</v>
       </c>
       <c r="B39" s="45"/>
-      <c r="C39" s="242" t="s">
+      <c r="C39" s="250" t="s">
         <v>18</v>
       </c>
-      <c r="D39" s="243"/>
+      <c r="D39" s="251"/>
       <c r="E39" s="66" t="s">
         <v>86</v>
       </c>
-      <c r="F39" s="242" t="s">
+      <c r="F39" s="250" t="s">
         <v>18</v>
       </c>
-      <c r="G39" s="243"/>
+      <c r="G39" s="251"/>
       <c r="H39" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="I39" s="242" t="s">
+      <c r="I39" s="250" t="s">
         <v>18</v>
       </c>
-      <c r="J39" s="243"/>
+      <c r="J39" s="251"/>
       <c r="K39" s="46"/>
       <c r="L39" s="4"/>
       <c r="M39" s="4"/>
@@ -4484,7 +4483,7 @@
       <c r="L44" s="5"/>
       <c r="M44" s="5"/>
     </row>
-    <row r="45" spans="1:13" ht="198">
+    <row r="45" spans="1:13" ht="91.5">
       <c r="A45" s="23" t="s">
         <v>101</v>
       </c>
@@ -4501,7 +4500,7 @@
         <v>103</v>
       </c>
       <c r="F45" s="86">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="G45" s="87">
         <f t="shared" si="4"/>
@@ -4619,10 +4618,10 @@
       <c r="M48" s="5"/>
     </row>
     <row r="49" spans="1:17" s="30" customFormat="1" ht="15.75">
-      <c r="A49" s="244" t="s">
+      <c r="A49" s="252" t="s">
         <v>26</v>
       </c>
-      <c r="B49" s="245"/>
+      <c r="B49" s="253"/>
       <c r="C49" s="71">
         <f>SUMPRODUCT(C40:C48,D40:D48)</f>
         <v>35.799999999999997</v>
@@ -4634,7 +4633,7 @@
       <c r="E49" s="59"/>
       <c r="F49" s="70">
         <f>SUMPRODUCT(F40:F48,G40:G48)</f>
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G49" s="51">
         <f>SUM(G40:G48)</f>
@@ -4658,28 +4657,28 @@
       <c r="Q49" s="44"/>
     </row>
     <row r="50" spans="1:17" ht="18.399999999999999" customHeight="1">
-      <c r="A50" s="249" t="s">
+      <c r="A50" s="257" t="s">
         <v>114</v>
       </c>
-      <c r="B50" s="249"/>
-      <c r="C50" s="242" t="s">
+      <c r="B50" s="257"/>
+      <c r="C50" s="250" t="s">
         <v>18</v>
       </c>
-      <c r="D50" s="243"/>
+      <c r="D50" s="251"/>
       <c r="E50" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="F50" s="242" t="s">
+      <c r="F50" s="250" t="s">
         <v>18</v>
       </c>
-      <c r="G50" s="243"/>
+      <c r="G50" s="251"/>
       <c r="H50" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="I50" s="242" t="s">
+      <c r="I50" s="250" t="s">
         <v>18</v>
       </c>
-      <c r="J50" s="243"/>
+      <c r="J50" s="251"/>
       <c r="K50" s="46"/>
       <c r="L50" s="8"/>
       <c r="M50" s="4"/>
@@ -4838,10 +4837,10 @@
       <c r="M55" s="5"/>
     </row>
     <row r="56" spans="1:17" s="44" customFormat="1" ht="15.75">
-      <c r="A56" s="244" t="s">
+      <c r="A56" s="252" t="s">
         <v>26</v>
       </c>
-      <c r="B56" s="245"/>
+      <c r="B56" s="253"/>
       <c r="C56" s="57">
         <f>SUMPRODUCT(C51:C55,D51:D55)</f>
         <v>8.5</v>
@@ -4873,27 +4872,27 @@
       <c r="M56" s="56"/>
     </row>
     <row r="57" spans="1:17" ht="18.75" customHeight="1">
-      <c r="A57" s="246" t="s">
+      <c r="A57" s="280" t="s">
         <v>2</v>
       </c>
-      <c r="B57" s="247"/>
-      <c r="C57" s="247"/>
-      <c r="D57" s="247"/>
-      <c r="E57" s="247"/>
-      <c r="F57" s="247"/>
-      <c r="G57" s="247"/>
-      <c r="H57" s="247"/>
-      <c r="I57" s="247"/>
-      <c r="J57" s="247"/>
-      <c r="K57" s="248"/>
+      <c r="B57" s="281"/>
+      <c r="C57" s="281"/>
+      <c r="D57" s="281"/>
+      <c r="E57" s="281"/>
+      <c r="F57" s="281"/>
+      <c r="G57" s="281"/>
+      <c r="H57" s="281"/>
+      <c r="I57" s="281"/>
+      <c r="J57" s="281"/>
+      <c r="K57" s="282"/>
       <c r="L57" s="4"/>
       <c r="M57" s="4"/>
     </row>
     <row r="58" spans="1:17">
-      <c r="A58" s="250" t="s">
+      <c r="A58" s="267" t="s">
         <v>129</v>
       </c>
-      <c r="B58" s="251"/>
+      <c r="B58" s="268"/>
       <c r="C58" s="34">
         <f>C11+C18+C22+C27+C32+C38+C49+C56</f>
         <v>79.199999999999989</v>
@@ -4905,7 +4904,7 @@
       <c r="E58" s="26"/>
       <c r="F58" s="35">
         <f>F11+F18+F22+F27+F32+F38+F49+F56</f>
-        <v>72.75</v>
+        <v>74.75</v>
       </c>
       <c r="G58" s="27">
         <f>G11+G18+G22+G27+G32+G38+G49+G56</f>
@@ -4925,33 +4924,68 @@
       <c r="M58" s="5"/>
     </row>
     <row r="59" spans="1:17" s="44" customFormat="1" ht="15.75">
-      <c r="A59" s="252" t="s">
+      <c r="A59" s="269" t="s">
         <v>130</v>
       </c>
-      <c r="B59" s="253"/>
-      <c r="C59" s="254">
+      <c r="B59" s="270"/>
+      <c r="C59" s="271">
         <f>C58/D58</f>
         <v>0.79199999999999993</v>
       </c>
-      <c r="D59" s="255"/>
-      <c r="E59" s="256"/>
-      <c r="F59" s="257">
+      <c r="D59" s="272"/>
+      <c r="E59" s="273"/>
+      <c r="F59" s="274">
         <f>F58/G58</f>
-        <v>0.72750000000000004</v>
-      </c>
-      <c r="G59" s="258"/>
-      <c r="H59" s="259"/>
-      <c r="I59" s="260">
+        <v>0.74750000000000005</v>
+      </c>
+      <c r="G59" s="275"/>
+      <c r="H59" s="276"/>
+      <c r="I59" s="277">
         <f>I58/J58</f>
         <v>0</v>
       </c>
-      <c r="J59" s="261"/>
-      <c r="K59" s="262"/>
+      <c r="J59" s="278"/>
+      <c r="K59" s="279"/>
       <c r="L59" s="72"/>
       <c r="M59" s="72"/>
     </row>
   </sheetData>
   <mergeCells count="51">
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A57:K57"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="I39:J39"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="I50:J50"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="C59:E59"/>
+    <mergeCell ref="F59:H59"/>
+    <mergeCell ref="I59:K59"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="N6:P6"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="I28:J28"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="A4:K4"/>
     <mergeCell ref="I6:K6"/>
@@ -4968,41 +5002,6 @@
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="F12:G12"/>
     <mergeCell ref="C8:D8"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="N6:P6"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="C59:E59"/>
-    <mergeCell ref="F59:H59"/>
-    <mergeCell ref="I59:K59"/>
-    <mergeCell ref="A57:K57"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="I39:J39"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="F50:G50"/>
-    <mergeCell ref="I50:J50"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A56:B56"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L18 L22 L27 L32 L38 L49 L11 C9:C10 F9:F10 I9:I10 C24:C26 F24:F26 I24:I26 C34:C37 F34:F37 I34:I37 C51:C55 F51:F55 I51:I55 I13:I17 F13:F17 C13:C17 I20:I21 F20:F21 C20:C21 I29:I31 F29:F31 C29:C31 I40:I48 F40:F48 C40:C48" xr:uid="{4A0D4DC8-F6F9-4765-AB49-E4E0ACDB1361}">
@@ -5024,7 +5023,7 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A2:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
@@ -6171,6 +6170,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B41E0342602C49449CD93109DBCAB8C5" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4cab946e3812a26735e8b0dc00d59aca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d3ea4e87-b30d-4ccc-9564-7710f23c54f0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="afa808ced5dc9827eedaaa69eb8b35dd" ns2:_="">
     <xsd:import namespace="d3ea4e87-b30d-4ccc-9564-7710f23c54f0"/>
@@ -6302,23 +6316,8 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CD1971BE-1E76-44E5-BF52-2DB1BB889C58}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F1A1E89-A0AE-4DED-85B2-2445C39C0F55}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6326,5 +6325,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F1A1E89-A0AE-4DED-85B2-2445C39C0F55}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CD1971BE-1E76-44E5-BF52-2DB1BB889C58}"/>
 </file>
</xml_diff>